<commit_message>
updating some bugs, adding more abilities
</commit_message>
<xml_diff>
--- a/data/DataGeneration_5_2024.xlsx
+++ b/data/DataGeneration_5_2024.xlsx
@@ -500,7 +500,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BK14"/>
+  <dimension ref="A1:BI14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -754,8 +754,6 @@
       <c r="BG1" s="10" t="n"/>
       <c r="BH1" s="1" t="n"/>
       <c r="BI1" s="1" t="n"/>
-      <c r="BJ1" s="1" t="n"/>
-      <c r="BK1" s="1" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="11" t="inlineStr">
@@ -1055,20 +1053,10 @@
       </c>
       <c r="BH2" s="11" t="inlineStr">
         <is>
-          <t>Unnamed: 57</t>
+          <t>New Project 1</t>
         </is>
       </c>
       <c r="BI2" s="11" t="inlineStr">
-        <is>
-          <t>Unnamed: 58</t>
-        </is>
-      </c>
-      <c r="BJ2" s="11" t="inlineStr">
-        <is>
-          <t>New Project 1</t>
-        </is>
-      </c>
-      <c r="BK2" s="11" t="inlineStr">
         <is>
           <t>New Project 2</t>
         </is>
@@ -1258,14 +1246,8 @@
       <c r="BG3" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="BH3" s="1" t="n">
-        <v/>
-      </c>
-      <c r="BI3" s="1" t="n">
-        <v/>
-      </c>
-      <c r="BJ3" s="1" t="n"/>
-      <c r="BK3" s="1" t="n"/>
+      <c r="BH3" s="1" t="n"/>
+      <c r="BI3" s="1" t="n"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -1451,14 +1433,8 @@
       <c r="BG4" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="BH4" s="1" t="n">
-        <v/>
-      </c>
-      <c r="BI4" s="1" t="n">
-        <v/>
-      </c>
-      <c r="BJ4" s="1" t="n"/>
-      <c r="BK4" s="1" t="n"/>
+      <c r="BH4" s="1" t="n"/>
+      <c r="BI4" s="1" t="n"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -1644,14 +1620,8 @@
       <c r="BG5" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="BH5" s="1" t="n">
-        <v/>
-      </c>
-      <c r="BI5" s="1" t="n">
-        <v/>
-      </c>
-      <c r="BJ5" s="1" t="n"/>
-      <c r="BK5" s="1" t="n"/>
+      <c r="BH5" s="1" t="n"/>
+      <c r="BI5" s="1" t="n"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -1837,14 +1807,8 @@
       <c r="BG6" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="BH6" s="1" t="n">
-        <v/>
-      </c>
-      <c r="BI6" s="1" t="n">
-        <v/>
-      </c>
-      <c r="BJ6" s="1" t="n"/>
-      <c r="BK6" s="1" t="n"/>
+      <c r="BH6" s="1" t="n"/>
+      <c r="BI6" s="1" t="n"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -2030,14 +1994,8 @@
       <c r="BG7" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="BH7" s="1" t="n">
-        <v/>
-      </c>
-      <c r="BI7" s="1" t="n">
-        <v>385.4</v>
-      </c>
-      <c r="BJ7" s="1" t="n"/>
-      <c r="BK7" s="1" t="n"/>
+      <c r="BH7" s="1" t="n"/>
+      <c r="BI7" s="1" t="n"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -2223,14 +2181,8 @@
       <c r="BG8" s="1" t="n">
         <v/>
       </c>
-      <c r="BH8" s="1" t="n">
-        <v/>
-      </c>
-      <c r="BI8" s="1" t="n">
-        <v/>
-      </c>
-      <c r="BJ8" s="1" t="n"/>
-      <c r="BK8" s="1" t="n"/>
+      <c r="BH8" s="1" t="n"/>
+      <c r="BI8" s="1" t="n"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
@@ -2416,14 +2368,8 @@
       <c r="BG9" s="1" t="n">
         <v/>
       </c>
-      <c r="BH9" s="1" t="n">
-        <v/>
-      </c>
-      <c r="BI9" s="1" t="n">
-        <v/>
-      </c>
-      <c r="BJ9" s="1" t="n"/>
-      <c r="BK9" s="1" t="n"/>
+      <c r="BH9" s="1" t="n"/>
+      <c r="BI9" s="1" t="n"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
@@ -2609,14 +2555,8 @@
       <c r="BG10" s="1" t="n">
         <v/>
       </c>
-      <c r="BH10" s="1" t="n">
-        <v/>
-      </c>
-      <c r="BI10" s="1" t="n">
-        <v/>
-      </c>
-      <c r="BJ10" s="1" t="n"/>
-      <c r="BK10" s="1" t="n"/>
+      <c r="BH10" s="1" t="n"/>
+      <c r="BI10" s="1" t="n"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
@@ -2802,14 +2742,8 @@
       <c r="BG11" s="1" t="n">
         <v/>
       </c>
-      <c r="BH11" s="1" t="n">
-        <v/>
-      </c>
-      <c r="BI11" s="1" t="n">
-        <v/>
-      </c>
-      <c r="BJ11" s="1" t="n"/>
-      <c r="BK11" s="1" t="n"/>
+      <c r="BH11" s="1" t="n"/>
+      <c r="BI11" s="1" t="n"/>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
@@ -2995,14 +2929,8 @@
       <c r="BG12" s="1" t="n">
         <v/>
       </c>
-      <c r="BH12" s="1" t="n">
-        <v/>
-      </c>
-      <c r="BI12" s="1" t="n">
-        <v/>
-      </c>
-      <c r="BJ12" s="1" t="n"/>
-      <c r="BK12" s="1" t="n"/>
+      <c r="BH12" s="1" t="n"/>
+      <c r="BI12" s="1" t="n"/>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
@@ -3188,14 +3116,8 @@
       <c r="BG13" s="1" t="n">
         <v/>
       </c>
-      <c r="BH13" s="1" t="n">
-        <v/>
-      </c>
-      <c r="BI13" s="1" t="n">
-        <v/>
-      </c>
-      <c r="BJ13" s="1" t="n"/>
-      <c r="BK13" s="1" t="n"/>
+      <c r="BH13" s="1" t="n"/>
+      <c r="BI13" s="1" t="n"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
@@ -3381,14 +3303,8 @@
       <c r="BG14" s="1" t="n">
         <v/>
       </c>
-      <c r="BH14" s="1" t="n">
-        <v/>
-      </c>
-      <c r="BI14" s="1" t="n">
-        <v/>
-      </c>
-      <c r="BJ14" s="1" t="n"/>
-      <c r="BK14" s="1" t="n"/>
+      <c r="BH14" s="1" t="n"/>
+      <c r="BI14" s="1" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>